<commit_message>
modify last point get condition
</commit_message>
<xml_diff>
--- a/src/main/resources/SH603976.xlsx
+++ b/src/main/resources/SH603976.xlsx
@@ -124,381 +124,311 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>20180116</t>
+          <t>20180207</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>2148.0</v>
+        <v>1376.0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>20180207</t>
+          <t>20180312</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>1376.0</v>
+        <v>1718.0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>20180312</t>
+          <t>20180326</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>1718.0</v>
+        <v>1431.0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>20180326</t>
+          <t>20180413</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>1431.0</v>
+        <v>2022.0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>20180413</t>
+          <t>20180423</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>2022.0</v>
+        <v>1671.0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>20180423</t>
+          <t>20180528</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>1671.0</v>
+        <v>2289.0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>20180528</t>
+          <t>20180706</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>2289.0</v>
+        <v>1482.0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>20180706</t>
+          <t>20180713</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>1482.0</v>
+        <v>1737.0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>20180713</t>
+          <t>20180824</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>1737.0</v>
+        <v>1383.0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>20180824</t>
+          <t>20180912</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>1383.0</v>
+        <v>1520.0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>20180912</t>
+          <t>20181012</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>1520.0</v>
+        <v>1124.0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>20181012</t>
+          <t>20181113</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>1124.0</v>
+        <v>1485.0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>20181113</t>
+          <t>20181126</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>1485.0</v>
+        <v>1323.0</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>20181126</t>
+          <t>20181211</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>1323.0</v>
+        <v>1941.0</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>20181211</t>
+          <t>20181228</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>1941.0</v>
+        <v>1622.0</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>20181228</t>
+          <t>20190109</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>1622.0</v>
+        <v>2041.0</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>20190109</t>
+          <t>20190130</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>2041.0</v>
+        <v>1642.0</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>20190130</t>
+          <t>20190225</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>1642.0</v>
+        <v>1968.0</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>20190225</t>
+          <t>20190311</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>1968.0</v>
+        <v>1692.0</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>20190311</t>
+          <t>20190319</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>1692.0</v>
+        <v>2216.0</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>20190319</t>
+          <t>20190606</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>2216.0</v>
+        <v>1430.0</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>20190606</t>
+          <t>20190724</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>1430.0</v>
+        <v>1808.0</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>20190724</t>
+          <t>20190812</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>1808.0</v>
+        <v>1383.0</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>20190812</t>
+          <t>20191121</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>1383.0</v>
+        <v>3392.0</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>20191023</t>
+          <t>20191230</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>2376.0</v>
+        <v>1680.0</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>20191028</t>
+          <t>20200121</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>2101.0</v>
+        <v>1865.0</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>20191121</t>
+          <t>20200204</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>3392.0</v>
+        <v>1355.0</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>20191230</t>
+          <t>20200225</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>1680.0</v>
+        <v>1978.0</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>20200121</t>
+          <t>20200319</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>1865.0</v>
+        <v>1451.0</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>20200204</t>
+          <t>20200521</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>1355.0</v>
+        <v>2700.0</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>20200225</t>
+          <t>20200529</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>1978.0</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>20200228</t>
-        </is>
-      </c>
-      <c r="B38" t="n">
-        <v>1651.0</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="inlineStr">
-        <is>
-          <t>20200306</t>
-        </is>
-      </c>
-      <c r="B39" t="n">
-        <v>1845.0</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="inlineStr">
-        <is>
-          <t>20200319</t>
-        </is>
-      </c>
-      <c r="B40" t="n">
-        <v>1451.0</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="inlineStr">
-        <is>
-          <t>20200428</t>
-        </is>
-      </c>
-      <c r="B41" t="n">
-        <v>1462.0</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="inlineStr">
-        <is>
-          <t>20200521</t>
-        </is>
-      </c>
-      <c r="B42" t="n">
-        <v>2700.0</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="inlineStr">
-        <is>
-          <t>20200529</t>
-        </is>
-      </c>
-      <c r="B43" t="n">
         <v>2015.0</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>20200624</t>
-        </is>
-      </c>
-      <c r="B44" t="n">
-        <v>3230.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix hour line out date bug
</commit_message>
<xml_diff>
--- a/src/main/resources/SH603976.xlsx
+++ b/src/main/resources/SH603976.xlsx
@@ -124,311 +124,331 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>20180207</t>
+          <t>20180116</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1376.0</v>
+        <v>2148.0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>20180312</t>
+          <t>20180207</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>1718.0</v>
+        <v>1376.0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>20180326</t>
+          <t>20180312</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>1431.0</v>
+        <v>1718.0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>20180413</t>
+          <t>20180326</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>2022.0</v>
+        <v>1431.0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>20180423</t>
+          <t>20180413</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>1671.0</v>
+        <v>2022.0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>20180528</t>
+          <t>20180423</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>2289.0</v>
+        <v>1671.0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>20180706</t>
+          <t>20180528</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>1482.0</v>
+        <v>2289.0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>20180713</t>
+          <t>20180706</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>1737.0</v>
+        <v>1482.0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>20180824</t>
+          <t>20180713</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>1383.0</v>
+        <v>1737.0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>20180912</t>
+          <t>20180824</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>1520.0</v>
+        <v>1383.0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>20181012</t>
+          <t>20180912</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>1124.0</v>
+        <v>1520.0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>20181113</t>
+          <t>20181012</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>1485.0</v>
+        <v>1124.0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>20181126</t>
+          <t>20181113</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>1323.0</v>
+        <v>1485.0</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>20181211</t>
+          <t>20181126</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>1941.0</v>
+        <v>1323.0</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>20181228</t>
+          <t>20181211</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>1622.0</v>
+        <v>1941.0</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>20190109</t>
+          <t>20181228</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>2041.0</v>
+        <v>1622.0</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>20190130</t>
+          <t>20190109</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>1642.0</v>
+        <v>2041.0</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>20190225</t>
+          <t>20190130</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>1968.0</v>
+        <v>1642.0</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>20190311</t>
+          <t>20190225</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>1692.0</v>
+        <v>1968.0</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>20190319</t>
+          <t>20190311</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>2216.0</v>
+        <v>1692.0</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>20190606</t>
+          <t>20190319</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>1430.0</v>
+        <v>2216.0</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>20190724</t>
+          <t>20190606</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>1808.0</v>
+        <v>1430.0</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>20190812</t>
+          <t>20190724</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>1383.0</v>
+        <v>1808.0</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>20191121</t>
+          <t>20190812</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>3392.0</v>
+        <v>1383.0</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>20191230</t>
+          <t>20191121</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>1680.0</v>
+        <v>3392.0</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>20200121</t>
+          <t>20191230</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>1865.0</v>
+        <v>1680.0</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>20200204</t>
+          <t>20200121</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>1355.0</v>
+        <v>1865.0</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>20200225</t>
+          <t>20200204</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>1978.0</v>
+        <v>1355.0</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>20200319</t>
+          <t>20200225</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>1451.0</v>
+        <v>1978.0</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>20200521</t>
+          <t>20200319</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>2700.0</v>
+        <v>1451.0</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
+          <t>20200521</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>2700.0</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
           <t>20200529</t>
         </is>
       </c>
-      <c r="B37" t="n">
+      <c r="B38" t="n">
         <v>2015.0</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>20200624</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>3230.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
left delete peak point bug fix
</commit_message>
<xml_diff>
--- a/src/main/resources/SH603976.xlsx
+++ b/src/main/resources/SH603976.xlsx
@@ -64,391 +64,401 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>20170904</t>
+          <t>20170822</t>
         </is>
       </c>
       <c r="B1" t="n">
-        <v>3433.0</v>
+        <v>1154.0</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>20170929</t>
+          <t>20170904</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>2308.0</v>
+        <v>3400.0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>20171013</t>
+          <t>20170929</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>2934.0</v>
+        <v>2275.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>20171206</t>
+          <t>20171013</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1728.0</v>
+        <v>2902.0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>20171228</t>
+          <t>20171206</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1993.0</v>
+        <v>1696.0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>20180108</t>
+          <t>20171228</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1844.0</v>
+        <v>1960.0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>20180116</t>
+          <t>20180108</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>2148.0</v>
+        <v>1812.0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>20180207</t>
+          <t>20180116</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>1376.0</v>
+        <v>2116.0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>20180312</t>
+          <t>20180207</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>1718.0</v>
+        <v>1344.0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>20180326</t>
+          <t>20180312</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>1431.0</v>
+        <v>1685.0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>20180413</t>
+          <t>20180326</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>2022.0</v>
+        <v>1398.0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>20180423</t>
+          <t>20180413</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>1671.0</v>
+        <v>1990.0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>20180528</t>
+          <t>20180423</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>2289.0</v>
+        <v>1639.0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>20180622</t>
+          <t>20180528</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>1492.0</v>
+        <v>2257.0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>20180713</t>
+          <t>20180706</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>1737.0</v>
+        <v>1450.0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>20181012</t>
+          <t>20180713</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>1124.0</v>
+        <v>1705.0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>20181113</t>
+          <t>20181012</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>1485.0</v>
+        <v>1092.0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>20181126</t>
+          <t>20181113</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>1323.0</v>
+        <v>1453.0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>20181211</t>
+          <t>20181126</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>1941.0</v>
+        <v>1291.0</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>20181228</t>
+          <t>20181211</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>1622.0</v>
+        <v>1909.0</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>20190109</t>
+          <t>20181228</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>2041.0</v>
+        <v>1590.0</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>20190130</t>
+          <t>20190109</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>1642.0</v>
+        <v>2009.0</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>20190225</t>
+          <t>20190130</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>1968.0</v>
+        <v>1610.0</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>20190311</t>
+          <t>20190225</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>1692.0</v>
+        <v>1936.0</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>20190319</t>
+          <t>20190311</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>2216.0</v>
+        <v>1660.0</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>20190606</t>
+          <t>20190319</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>1430.0</v>
+        <v>2184.0</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>20190724</t>
+          <t>20190606</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>1808.0</v>
+        <v>1398.0</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>20190812</t>
+          <t>20190724</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>1383.0</v>
+        <v>1776.0</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>20191121</t>
+          <t>20190812</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>3392.0</v>
+        <v>1351.0</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>20191230</t>
+          <t>20191121</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>1680.0</v>
+        <v>3360.0</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>20200121</t>
+          <t>20191230</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>1865.0</v>
+        <v>1648.0</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>20200204</t>
+          <t>20200121</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>1355.0</v>
+        <v>1833.0</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>20200225</t>
+          <t>20200204</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>1978.0</v>
+        <v>1323.0</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>20200319</t>
+          <t>20200225</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>1451.0</v>
+        <v>1946.0</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>20200327</t>
+          <t>20200319</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>1665.0</v>
+        <v>1419.0</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>20200402</t>
+          <t>20200327</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>1505.0</v>
+        <v>1800.0</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>20200521</t>
+          <t>20200428</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>2700.0</v>
+        <v>1430.0</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>20200529</t>
+          <t>20200521</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>2015.0</v>
+        <v>2668.0</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>20200624</t>
+          <t>20200529</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>3230.0</v>
+        <v>1983.0</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>20200804</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>10800.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>